<commit_message>
Sprint 8 | maj
</commit_message>
<xml_diff>
--- a/doc/organisation/Burndown Chart/Sprint 8.xlsx
+++ b/doc/organisation/Burndown Chart/Sprint 8.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\castrignano.vincenzo\Documents\Cours\2e_annee\Github\BSN_2024\doc\organisation\Burndown Chart\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB52F839-3A0D-4191-B9E1-DB3DDF26DF18}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C3F354C-09BD-47EC-97A3-6A9B5252EB2D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9060" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -621,10 +621,10 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>0</c:v>
@@ -782,49 +782,49 @@
                   <c:v>40</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>40</c:v>
+                  <c:v>39</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>40</c:v>
+                  <c:v>37</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>40</c:v>
+                  <c:v>37</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>40</c:v>
+                  <c:v>37</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>40</c:v>
+                  <c:v>37</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>40</c:v>
+                  <c:v>37</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>40</c:v>
+                  <c:v>37</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>40</c:v>
+                  <c:v>37</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>40</c:v>
+                  <c:v>37</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>40</c:v>
+                  <c:v>37</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>40</c:v>
+                  <c:v>37</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>40</c:v>
+                  <c:v>37</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>40</c:v>
+                  <c:v>37</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>40</c:v>
+                  <c:v>37</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>40</c:v>
+                  <c:v>37</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1598,7 +1598,7 @@
   <dimension ref="A1:R12"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A22" sqref="A17:A22"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14"/>
@@ -1672,10 +1672,10 @@
         <v>10</v>
       </c>
       <c r="C2" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D2" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E2" s="4">
         <v>0</v>
@@ -1718,7 +1718,7 @@
       </c>
       <c r="R2" s="3">
         <f>B2-(SUM(C2:Q2))</f>
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:18" ht="14.5">
@@ -1789,7 +1789,7 @@
         <v>0</v>
       </c>
       <c r="D4" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E4" s="4">
         <v>0</v>
@@ -1832,7 +1832,7 @@
       </c>
       <c r="R4" s="3">
         <f t="shared" si="0"/>
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="5" spans="1:18" ht="14.5">
@@ -1922,59 +1922,59 @@
         <v>1.4285714285714286</v>
       </c>
       <c r="D9" s="8">
-        <f>SUM($B$2:$B$5)/28</f>
+        <f t="shared" ref="D9:Q9" si="1">SUM($B$2:$B$5)/28</f>
         <v>1.4285714285714286</v>
       </c>
       <c r="E9" s="8">
-        <f>SUM($B$2:$B$5)/28</f>
+        <f t="shared" si="1"/>
         <v>1.4285714285714286</v>
       </c>
       <c r="F9" s="8">
-        <f>SUM($B$2:$B$5)/28</f>
+        <f t="shared" si="1"/>
         <v>1.4285714285714286</v>
       </c>
       <c r="G9" s="8">
-        <f>SUM($B$2:$B$5)/28</f>
+        <f t="shared" si="1"/>
         <v>1.4285714285714286</v>
       </c>
       <c r="H9" s="8">
-        <f>SUM($B$2:$B$5)/28</f>
+        <f t="shared" si="1"/>
         <v>1.4285714285714286</v>
       </c>
       <c r="I9" s="8">
-        <f>SUM($B$2:$B$5)/28</f>
+        <f t="shared" si="1"/>
         <v>1.4285714285714286</v>
       </c>
       <c r="J9" s="8">
-        <f>SUM($B$2:$B$5)/28</f>
+        <f t="shared" si="1"/>
         <v>1.4285714285714286</v>
       </c>
       <c r="K9" s="8">
-        <f>SUM($B$2:$B$5)/28</f>
+        <f t="shared" si="1"/>
         <v>1.4285714285714286</v>
       </c>
       <c r="L9" s="8">
-        <f>SUM($B$2:$B$5)/28</f>
+        <f t="shared" si="1"/>
         <v>1.4285714285714286</v>
       </c>
       <c r="M9" s="8">
-        <f>SUM($B$2:$B$5)/28</f>
+        <f t="shared" si="1"/>
         <v>1.4285714285714286</v>
       </c>
       <c r="N9" s="8">
-        <f>SUM($B$2:$B$5)/28</f>
+        <f t="shared" si="1"/>
         <v>1.4285714285714286</v>
       </c>
       <c r="O9" s="8">
-        <f>SUM($B$2:$B$5)/28</f>
+        <f t="shared" si="1"/>
         <v>1.4285714285714286</v>
       </c>
       <c r="P9" s="8">
-        <f>SUM($B$2:$B$5)/28</f>
+        <f t="shared" si="1"/>
         <v>1.4285714285714286</v>
       </c>
       <c r="Q9" s="8">
-        <f>SUM($B$2:$B$5)/28</f>
+        <f t="shared" si="1"/>
         <v>1.4285714285714286</v>
       </c>
     </row>
@@ -1986,63 +1986,63 @@
         <v>0</v>
       </c>
       <c r="C10" s="10">
-        <f>SUM(C2:C5)</f>
-        <v>0</v>
+        <f t="shared" ref="C10:Q10" si="2">SUM(C2:C5)</f>
+        <v>1</v>
       </c>
       <c r="D10" s="10">
-        <f>SUM(D2:D5)</f>
-        <v>0</v>
+        <f t="shared" si="2"/>
+        <v>2</v>
       </c>
       <c r="E10" s="10">
-        <f>SUM(E2:E5)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="F10" s="10">
-        <f>SUM(F2:F5)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="G10" s="10">
-        <f>SUM(G2:G5)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="H10" s="10">
-        <f>SUM(H2:H5)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="I10" s="10">
-        <f>SUM(I2:I5)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="J10" s="10">
-        <f>SUM(J2:J5)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="K10" s="10">
-        <f>SUM(K2:K5)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="L10" s="10">
-        <f>SUM(L2:L5)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="M10" s="10">
-        <f>SUM(M2:M5)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="N10" s="10">
-        <f>SUM(N2:N5)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="O10" s="10">
-        <f>SUM(O2:O5)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="P10" s="10">
-        <f>SUM(P2:P5)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="Q10" s="10">
-        <f>SUM(Q2:Q5)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
@@ -2055,64 +2055,64 @@
         <v>40</v>
       </c>
       <c r="C11" s="8">
-        <f t="shared" ref="C11:AD11" si="1">B11-C10</f>
-        <v>40</v>
+        <f t="shared" ref="C11:Q11" si="3">B11-C10</f>
+        <v>39</v>
       </c>
       <c r="D11" s="8">
-        <f t="shared" si="1"/>
-        <v>40</v>
+        <f t="shared" si="3"/>
+        <v>37</v>
       </c>
       <c r="E11" s="8">
-        <f t="shared" si="1"/>
-        <v>40</v>
+        <f t="shared" si="3"/>
+        <v>37</v>
       </c>
       <c r="F11" s="8">
-        <f t="shared" si="1"/>
-        <v>40</v>
+        <f t="shared" si="3"/>
+        <v>37</v>
       </c>
       <c r="G11" s="8">
-        <f t="shared" si="1"/>
-        <v>40</v>
+        <f t="shared" si="3"/>
+        <v>37</v>
       </c>
       <c r="H11" s="8">
-        <f t="shared" si="1"/>
-        <v>40</v>
+        <f t="shared" si="3"/>
+        <v>37</v>
       </c>
       <c r="I11" s="8">
-        <f t="shared" si="1"/>
-        <v>40</v>
+        <f t="shared" si="3"/>
+        <v>37</v>
       </c>
       <c r="J11" s="8">
-        <f t="shared" si="1"/>
-        <v>40</v>
+        <f t="shared" si="3"/>
+        <v>37</v>
       </c>
       <c r="K11" s="8">
-        <f t="shared" si="1"/>
-        <v>40</v>
+        <f t="shared" si="3"/>
+        <v>37</v>
       </c>
       <c r="L11" s="8">
-        <f t="shared" si="1"/>
-        <v>40</v>
+        <f t="shared" si="3"/>
+        <v>37</v>
       </c>
       <c r="M11" s="8">
-        <f t="shared" si="1"/>
-        <v>40</v>
+        <f t="shared" si="3"/>
+        <v>37</v>
       </c>
       <c r="N11" s="8">
-        <f t="shared" si="1"/>
-        <v>40</v>
+        <f t="shared" si="3"/>
+        <v>37</v>
       </c>
       <c r="O11" s="8">
-        <f t="shared" si="1"/>
-        <v>40</v>
+        <f t="shared" si="3"/>
+        <v>37</v>
       </c>
       <c r="P11" s="8">
-        <f t="shared" si="1"/>
-        <v>40</v>
+        <f t="shared" si="3"/>
+        <v>37</v>
       </c>
       <c r="Q11" s="8">
-        <f t="shared" si="1"/>
-        <v>40</v>
+        <f t="shared" si="3"/>
+        <v>37</v>
       </c>
     </row>
     <row r="12" spans="1:18" ht="14.5">
@@ -2124,63 +2124,63 @@
         <v>40</v>
       </c>
       <c r="C12" s="13">
-        <f t="shared" ref="C12:AD12" si="2">B12-C9</f>
+        <f t="shared" ref="C12:Q12" si="4">B12-C9</f>
         <v>38.571428571428569</v>
       </c>
       <c r="D12" s="13">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>37.142857142857139</v>
       </c>
       <c r="E12" s="13">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>35.714285714285708</v>
       </c>
       <c r="F12" s="13">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>34.285714285714278</v>
       </c>
       <c r="G12" s="13">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>32.857142857142847</v>
       </c>
       <c r="H12" s="13">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>31.42857142857142</v>
       </c>
       <c r="I12" s="13">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>29.999999999999993</v>
       </c>
       <c r="J12" s="13">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>28.571428571428566</v>
       </c>
       <c r="K12" s="13">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>27.142857142857139</v>
       </c>
       <c r="L12" s="13">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>25.714285714285712</v>
       </c>
       <c r="M12" s="13">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>24.285714285714285</v>
       </c>
       <c r="N12" s="13">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>22.857142857142858</v>
       </c>
       <c r="O12" s="13">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>21.428571428571431</v>
       </c>
       <c r="P12" s="13">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>20.000000000000004</v>
       </c>
       <c r="Q12" s="13">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>18.571428571428577</v>
       </c>
     </row>

</xml_diff>